<commit_message>
training trials stimuli replaced
</commit_message>
<xml_diff>
--- a/html/resources/trainingtrials_nonsocial.xlsx
+++ b/html/resources/trainingtrials_nonsocial.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raimundbuehler/Desktop/RALT_english/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raimundbuehler/Desktop/RALT_PLD_english/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C51F4F8-BD4E-F649-BB12-95A94C755FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BECBEB6-23E9-D244-9183-1808704B3A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="1060" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Stim</t>
   </si>
@@ -76,43 +76,16 @@
     <t>Mandalas/Angry/Angry_blur/02_angry_blur.mp4</t>
   </si>
   <si>
-    <t>Mandalas_new/neutral/Mandala3_neutral.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/happy/Mandala3_happy.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/angry/Mandala3_angry.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/neutral/Mandala2_neutral.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/happy/Mandala2_happy.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/angry/Mandala2_angry.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/neutral/Mandala4_neutral.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/happy/Mandala4_happy.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/angry/Mandala4_angry.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/neutral/Mandala1_neutral.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/happy/Mandala1_happy.mp4</t>
-  </si>
-  <si>
-    <t>Mandalas_new/angry/Mandala1_angry.mp4</t>
-  </si>
-  <si>
     <t>CorrCatTrain</t>
+  </si>
+  <si>
+    <t>Stimuli/neutral/Still.jpg</t>
+  </si>
+  <si>
+    <t>Stimuli/nonsocial/Right Tick.mp4</t>
+  </si>
+  <si>
+    <t>Stimuli/nonsocial/Wrong Tick.mp4</t>
   </si>
 </sst>
 </file>
@@ -492,7 +465,7 @@
   <dimension ref="A1:L91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -525,13 +498,13 @@
         <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -543,13 +516,13 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -561,13 +534,13 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -580,13 +553,13 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>

</xml_diff>